<commit_message>
added new custom script to add or update values in location entity
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\temp_projects\json_values_checker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B7B7240-5B72-4B09-A947-B83A4CDD832C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A168FDF3-48CD-4F21-A969-26F5AA4ED587}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{662C8D38-9D08-4E92-B397-10311D5A8703}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -427,7 +428,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -498,4 +499,16 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00FE0482-5410-4B9D-B200-8E7C7DC27E31}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>